<commit_message>
Further improve wink detection
</commit_message>
<xml_diff>
--- a/status.xlsx
+++ b/status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Expected</t>
   </si>
@@ -42,28 +42,31 @@
     <t>Setting</t>
   </si>
   <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; cascades/Mouth.xml</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 1.2 &amp;&amp; mn = 3</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 2 &amp;&amp; mn = 5</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 1.8 &amp;&amp; mn = 3</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 1.8 &amp;&amp; mn = 2</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 2 &amp;&amp; mn = 2</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 2 &amp;&amp; mn = 2 &amp;&amp; custom gf</t>
-  </si>
-  <si>
-    <t>haarcascade_frontalface_default.xml &amp;&amp; haarcascade_eye.xml &amp;&amp; sf = 2 &amp;&amp; mn = 1</t>
+    <t>sf = 1.2, mn = 3, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 2, mn = 5, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 1.8, mn = 3, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 1.8, mn = 2, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 2, mn = 2, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 2, mn = 1, ms = (30,60)</t>
+  </si>
+  <si>
+    <t>sf = 2, mn = 1, ms = (40,60)</t>
+  </si>
+  <si>
+    <t>sf = 2, mn = 1, ms = (60,60)</t>
+  </si>
+  <si>
+    <t>Default cascades</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -131,12 +134,43 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -411,15 +445,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="82.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
@@ -444,179 +670,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="58.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>